<commit_message>
Add geography query for map
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\FIZZ\Documents\@MOOC\@ Udacity PDSP\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\FIZZ\Documents\@MOOC\@ Udacity PDSP\Projects\SQL\Sakila Database - Udacity SQL Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475C1C0D-403A-492B-8A08-1C14D3B94A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886FDDBE-7351-4A24-95E8-8C67985C1D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13260" tabRatio="655" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13260" tabRatio="655" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1-1 " sheetId="1" r:id="rId1"/>
@@ -21,19 +21,20 @@
     <sheet name="Suggestion3" sheetId="6" r:id="rId6"/>
     <sheet name="Question 3" sheetId="7" r:id="rId7"/>
     <sheet name="Suggestion4" sheetId="8" r:id="rId8"/>
+    <sheet name="Question 4" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="2" r:id="rId11"/>
-    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId12"/>
+    <pivotCache cacheId="3" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="516">
   <si>
     <t>film_title</t>
   </si>
@@ -1257,6 +1258,340 @@
   </si>
   <si>
     <t>Rental count</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>rentals</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Yugoslavia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Kazakstan</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Congo, The Democratic Republic of the</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Runion</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Holy See (Vatican City State)</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Virgin Islands, U.S.</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>French Guiana</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Question 4: Where should the customer accquisition funds should be spent to increase
+the rentals?</t>
   </si>
 </sst>
 </file>
@@ -1740,7 +2075,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1758,6 +2093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14919,7 +15255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -15066,4 +15402,896 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52C0328-434A-4F44-A875-A035A502D05E}">
+  <dimension ref="A1:B110"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B5" s="5">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="5">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B7" s="5">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B8" s="5">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B9" s="5">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B10" s="5">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B11" s="5">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B12" s="5">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="5">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" s="5">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B15" s="5">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B16" s="5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B17" s="5">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B18" s="5">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B19" s="5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B20" s="5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B21" s="5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B22" s="5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B23" s="5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B24" s="5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B25" s="5">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B26" s="5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B27" s="5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B28" s="5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="B29" s="5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B30" s="5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B31" s="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B32" s="5">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B33" s="5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B34" s="5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B35" s="5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B36" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B37" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B38" s="5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="B39" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B40" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B42" s="5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B43" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B44" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B45" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B46" s="5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B47" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B48" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B49" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B50" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B51" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B52" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B53" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="B54" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B55" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="B56" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B57" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B58" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B59" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B60" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B61" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="B62" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B63" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B64" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B65" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="B66" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B67" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B68" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="B69" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B70" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B71" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B72" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B73" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B74" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B75" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="B76" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B77" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="B78" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="B79" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="B80" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B81" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B82" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B83" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B84" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B85" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B86" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B87" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B88" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B89" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B90" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B91" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B92" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B93" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B94" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B95" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B96" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B97" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="B98" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="B99" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B100" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="B101" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B102" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B103" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B104" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B105" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B106" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B107" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B108" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B109" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B110" s="5">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>